<commit_message>
renamed one of the sheets
</commit_message>
<xml_diff>
--- a/s3_quality_data.xlsx
+++ b/s3_quality_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strength/Documents/DepenD Lab/NeuroMAP/NMAPReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2D968AA-B5B4-F64D-B22E-88AC23DD86E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92336B36-C691-024C-B270-2CAB6C033AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" activeTab="5" xr2:uid="{B95E2433-AFE6-134A-A26B-17E15D2DB442}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{B95E2433-AFE6-134A-A26B-17E15D2DB442}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="S3_Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Vanilla Baseline" sheetId="2" r:id="rId2"/>
     <sheet name="Neighborhood Notes" sheetId="3" r:id="rId3"/>
     <sheet name="Vending Machine Notes" sheetId="4" r:id="rId4"/>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6FF9413-7558-704E-A40A-D5EC03B7F1A3}">
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
@@ -6978,7 +6978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D3043F-A3F4-124B-BC95-99506BA51244}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D55"/>
     </sheetView>
   </sheetViews>

</xml_diff>